<commit_message>
Updated upto 4 th june
</commit_message>
<xml_diff>
--- a/april/WT_2021_April_PRSSVRAJU Master File.xlsx
+++ b/april/WT_2021_April_PRSSVRAJU Master File.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pothuriraju/Documents/Attandance Format/2021/Wt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pothuriraju/Documents/Attandance Format/2021/Raghu WT/april/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BEE9A6-0E5F-354A-90C9-2465C07FDF1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6576D9A8-DAAD-2D4A-A9CE-A10C18733A2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="500" windowWidth="32540" windowHeight="19500" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2057,27 +2057,7 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3739,7 +3719,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="13" priority="1" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1" stopIfTrue="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -8497,7 +8477,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D117">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13261,7 +13241,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D125">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18103,7 +18083,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D125">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22837,7 +22817,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D121:D125">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22847,8 +22827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E6B8F9-45BD-1647-8AFD-81718C3D0A4C}">
   <dimension ref="B4:H204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30002,7 +29982,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D43">
-    <cfRule type="duplicateValues" dxfId="12" priority="1" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1" stopIfTrue="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -31385,7 +31365,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D35">
-    <cfRule type="duplicateValues" dxfId="11" priority="1" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1" stopIfTrue="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -32894,7 +32874,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D44">
-    <cfRule type="duplicateValues" dxfId="10" priority="1" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1" stopIfTrue="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -37687,7 +37667,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D43">
-    <cfRule type="duplicateValues" dxfId="9" priority="1" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1" stopIfTrue="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -42368,7 +42348,7 @@
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="D5:D43">
-    <cfRule type="duplicateValues" dxfId="8" priority="1" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1" stopIfTrue="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -47084,7 +47064,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D117">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>